<commit_message>
Adding firms with no mentions as an intensity of 0
</commit_message>
<xml_diff>
--- a/Batch_A_Report.xlsx
+++ b/Batch_A_Report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
         <v>6281</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3674999999999999</v>
+        <v>0.3129842553139992</v>
       </c>
       <c r="C2" t="n">
         <v>1632</v>
@@ -479,113 +479,113 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>50863</v>
+        <v>40730</v>
       </c>
       <c r="B3" t="n">
-        <v>10.5145</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>6008</v>
+        <v>12206</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>INTEL CORP</t>
+          <t>DIRECTV GROUP INC</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.0157174840569496</v>
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>334119</t>
+          <t>334416</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>106040</v>
+        <v>50863</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8959999999999999</v>
+        <v>0.2443607110705934</v>
       </c>
       <c r="C4" t="n">
-        <v>11399</v>
+        <v>6008</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>WESTERN DIGITAL CORP</t>
+          <t>INTEL CORP</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.009449694305658301</v>
+        <v>0.0157174840569496</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>334118</t>
+          <t>334119</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>723125</v>
+        <v>65011</v>
       </c>
       <c r="B5" t="n">
-        <v>10.0422</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>7343</v>
+        <v>7260</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MICRON TECHNOLOGY INC</t>
+          <t>MEREDITH CORP</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.0063047283329069</v>
+        <v>0.0014044943964108</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>519130</t>
+          <t>334210</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>789019</v>
+        <v>70415</v>
       </c>
       <c r="B6" t="n">
-        <v>20.043</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>12141</v>
+        <v>7759</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>MICROSOFT CORP</t>
+          <t>GP STRATEGIES CORP</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.0242415703833103</v>
+        <v>0.0015037594130262</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>999990</t>
+          <t>519130</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>792130</v>
+        <v>78749</v>
       </c>
       <c r="B7" t="n">
-        <v>6.391599999999999</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>25320</v>
+        <v>8599</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DATAWATCH CORP</t>
+          <t>AGILYSYS INC</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -593,71 +593,71 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>511210</t>
+          <t>541512</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>796343</v>
+        <v>106040</v>
       </c>
       <c r="B8" t="n">
-        <v>4.5241</v>
+        <v>0.63974640383283</v>
       </c>
       <c r="C8" t="n">
-        <v>12540</v>
+        <v>11399</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ADOBE SYSTEMS INC</t>
+          <t>WESTERN DIGITAL CORP</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.0239260476082563</v>
+        <v>0.009449694305658301</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>451110</t>
+          <t>334118</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>798354</v>
+        <v>320193</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5669999999999999</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>12635</v>
+        <v>1690</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>FISERV INC</t>
+          <t>APPLE INC</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.0002362949016969</v>
+        <v>0.0133301597088575</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>334111</t>
+          <t>336111</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>814547</v>
+        <v>700841</v>
       </c>
       <c r="B10" t="n">
-        <v>18.8021</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>13824</v>
+        <v>8892</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>FAIR ISAAC CORP</t>
+          <t>RCM TECHNOLOGIES INC</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -671,65 +671,65 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>857005</v>
+        <v>714603</v>
       </c>
       <c r="B11" t="n">
-        <v>4.4575</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>18699</v>
+        <v>3707</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>PARAMETRIC TECHNOLOGY CORP</t>
+          <t>DST SYSTEMS INC</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.0051993066444993</v>
+        <v>0.000891265575774</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>334210</t>
+          <t>334419</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>858877</v>
+        <v>723125</v>
       </c>
       <c r="B12" t="n">
-        <v>4.7</v>
+        <v>0.2668582551509522</v>
       </c>
       <c r="C12" t="n">
-        <v>20779</v>
+        <v>7343</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CISCO SYSTEMS INC</t>
+          <t>MICRON TECHNOLOGY INC</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.0061595761217176</v>
+        <v>0.0063047283329069</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>519130</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>884144</v>
+        <v>751978</v>
       </c>
       <c r="B13" t="n">
-        <v>1.099</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>25138</v>
+        <v>21238</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>FORGENT NETWORKS INC</t>
+          <t>VICOR CORP</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -737,47 +737,47 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>541512</t>
+          <t>334113</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>896878</v>
+        <v>789019</v>
       </c>
       <c r="B14" t="n">
-        <v>0.7559999999999999</v>
+        <v>0.1523283981628243</v>
       </c>
       <c r="C14" t="n">
-        <v>27928</v>
+        <v>12141</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>INTUIT INC</t>
+          <t>MICROSOFT CORP</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.0137825421988964</v>
+        <v>0.0242415703833103</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>337127</t>
+          <t>999990</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>903651</v>
+        <v>792130</v>
       </c>
       <c r="B15" t="n">
-        <v>0.9720000000000001</v>
+        <v>0.1666953516934278</v>
       </c>
       <c r="C15" t="n">
-        <v>28717</v>
+        <v>25320</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>INNODATA ISOGEN INC</t>
+          <t>DATAWATCH CORP</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -785,151 +785,847 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>519130</t>
+          <t>511210</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>935036</v>
+        <v>794323</v>
       </c>
       <c r="B16" t="n">
-        <v>1.44</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>31564</v>
+        <v>13440</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>TRNSACTN SYS ARCHTCTS  -CL A</t>
+          <t>LEVEL 3 COMMUNICATIONS INC</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.0013386880746111</v>
+        <v>0.0006079027079977</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>518210</t>
+          <t>519130</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1036188</v>
+        <v>796343</v>
       </c>
       <c r="B17" t="n">
-        <v>1.792</v>
+        <v>0.427280084551808</v>
       </c>
       <c r="C17" t="n">
-        <v>65226</v>
+        <v>12540</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>QAD INC</t>
+          <t>ADOBE SYSTEMS INC</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>0.0239260476082563</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>511210</t>
+          <t>451110</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1108524</v>
+        <v>798354</v>
       </c>
       <c r="B18" t="n">
-        <v>12.4983</v>
+        <v>0.4491629633738837</v>
       </c>
       <c r="C18" t="n">
-        <v>157855</v>
+        <v>12635</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>SALESFORCE.COM INC</t>
+          <t>FISERV INC</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.0081739416345953</v>
+        <v>0.0002362949016969</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>325414</t>
+          <t>334111</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1130713</v>
+        <v>814547</v>
       </c>
       <c r="B19" t="n">
-        <v>2.024</v>
+        <v>0.1866117495426576</v>
       </c>
       <c r="C19" t="n">
-        <v>147868</v>
+        <v>13824</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>OVERSTOCK.COM INC</t>
+          <t>FAIR ISAAC CORP</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.015358361415565</v>
+        <v>0</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>511210</t>
+          <t>541512</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1341439</v>
+        <v>828146</v>
       </c>
       <c r="B20" t="n">
-        <v>3.94</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>12142</v>
+        <v>28374</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ORACLE CORP</t>
+          <t>INTERLINK ELECTRONICS</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.0071220458485186</v>
+        <v>0</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>561990</t>
+          <t>518210</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1652044</v>
+        <v>849547</v>
       </c>
       <c r="B21" t="n">
-        <v>5.306299999999999</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>160329</v>
+        <v>26012</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>GOOGLE INC</t>
+          <t>BLACK BOX CORP</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.0297704450786113</v>
+        <v>0</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>334111</t>
+          <t>511210</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>857005</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.5656636031473207</v>
+      </c>
+      <c r="C22" t="n">
+        <v>18699</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>PARAMETRIC TECHNOLOGY CORP</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0051993066444993</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>334210</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>858877</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.4351165437101261</v>
+      </c>
+      <c r="C23" t="n">
+        <v>20779</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>CISCO SYSTEMS INC</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0061595761217176</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>866729</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>5349</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>GROLIER INC</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>519130</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>882835</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>64423</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>DELTEK SYSTEMS INC</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>334413</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>884144</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.741461040838496</v>
+      </c>
+      <c r="C26" t="n">
+        <v>25138</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>FORGENT NETWORKS INC</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>541512</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>896841</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>27925</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>AVID TECHNOLOGY INC</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>0.005167958792299</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>334220</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>896878</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.1407596238032312</v>
+      </c>
+      <c r="C28" t="n">
+        <v>27928</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>INTUIT INC</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0137825421988964</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>337127</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>903651</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.6790482561804437</v>
+      </c>
+      <c r="C29" t="n">
+        <v>28717</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>INNODATA ISOGEN INC</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>519130</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>909494</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>62723</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>TUCOWS INC</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>334413</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>912093</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>29241</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>JDS UNIPHASE CORP</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>334413</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>935036</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.8919980393051106</v>
+      </c>
+      <c r="C32" t="n">
+        <v>31564</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>TRNSACTN SYS ARCHTCTS  -CL A</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>0.0013386880746111</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>518210</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>943034</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>31775</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>IMAGE SENSING SYSTEMS INC</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>334419</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1014111</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>7244</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>MEMOREX CORP</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>51121</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1018724</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>64768</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>AMAZON.COM INC</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>0.0122375879436731</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1024478</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>9203</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>ROCKWELL AUTOMATION</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0.0007662835414521</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>541512</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1029744</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>109186</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>SONIC FOUNDRY INC</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>334119</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1036188</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.513379092450063</v>
+      </c>
+      <c r="C38" t="n">
+        <v>65226</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>QAD INC</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>511210</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1038222</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>64850</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>REIS INC</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>519130</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1065280</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>147579</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>NETFLIX INC</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>0.0133382733911275</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>332721</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1078099</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>121662</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>QUEPASA CORP</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>541512</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1087423</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>122841</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>RED HAT INC</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>0.0047281323932111</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>334119</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1108524</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.2001972116607018</v>
+      </c>
+      <c r="C43" t="n">
+        <v>157855</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>SALESFORCE.COM INC</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>0.0081739416345953</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>325414</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1130713</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.3688601527724288</v>
+      </c>
+      <c r="C44" t="n">
+        <v>147868</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>OVERSTOCK.COM INC</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>0.015358361415565</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>511210</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1157817</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>149360</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>HOSTING SITE NETWORK INC</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>334413</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1296445</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>160913</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>ORMAT TECHNOLOGIES INC</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>511210</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1341439</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.5324551103999438</v>
+      </c>
+      <c r="C47" t="n">
+        <v>12142</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>ORACLE CORP</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>0.0071220458485186</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>561990</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1561880</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>114242</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>WHITNEY INFORMATION NET INC</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>541519</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1633917</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>145471</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>PAYPAL INC</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>334310</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1645494</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>28853</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>ARRIS GROUP INC</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>0.0011198208667337</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>511210</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Every new run with AI will save restults to a new file with auto number suffix. Validation script now takes an aifile argument with the AI results file name.
</commit_message>
<xml_diff>
--- a/Batch_A_Report.xlsx
+++ b/Batch_A_Report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
         <v>6281</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3129842553139992</v>
+        <v>0.03101405352916946</v>
       </c>
       <c r="C2" t="n">
         <v>1632</v>
@@ -479,17 +479,17 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>40730</v>
+        <v>23197</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>12206</v>
+        <v>138613</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>DIRECTV GROUP INC</t>
+          <t>TELECOMMUNICATION SYS INC</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -497,407 +497,407 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>334416</t>
+          <t>541512</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>50863</v>
+        <v>40730</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2443607110705934</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>6008</v>
+        <v>12206</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>INTEL CORP</t>
+          <t>DIRECTV GROUP INC</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.0157174840569496</v>
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>334119</t>
+          <t>334416</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>65011</v>
+        <v>50863</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.2443607110705934</v>
       </c>
       <c r="C5" t="n">
-        <v>7260</v>
+        <v>6008</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MEREDITH CORP</t>
+          <t>INTEL CORP</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.0014044943964108</v>
+        <v>0.0157174840569496</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>334210</t>
+          <t>334119</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>70415</v>
+        <v>65011</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>7759</v>
+        <v>7260</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>GP STRATEGIES CORP</t>
+          <t>MEREDITH CORP</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.0015037594130262</v>
+        <v>0.0014044943964108</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>519130</t>
+          <t>334210</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>78749</v>
+        <v>70415</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>8599</v>
+        <v>7759</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>AGILYSYS INC</t>
+          <t>GP STRATEGIES CORP</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.0015037594130262</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>541512</t>
+          <t>519130</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>106040</v>
+        <v>78749</v>
       </c>
       <c r="B8" t="n">
-        <v>0.63974640383283</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>11399</v>
+        <v>8599</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>WESTERN DIGITAL CORP</t>
+          <t>AGILYSYS INC</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.009449694305658301</v>
+        <v>0</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>334118</t>
+          <t>541512</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>320193</v>
+        <v>106040</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.63974640383283</v>
       </c>
       <c r="C9" t="n">
-        <v>1690</v>
+        <v>11399</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>APPLE INC</t>
+          <t>WESTERN DIGITAL CORP</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.0133301597088575</v>
+        <v>0.009449694305658301</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>336111</t>
+          <t>334118</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>700841</v>
+        <v>320193</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>8892</v>
+        <v>1690</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>RCM TECHNOLOGIES INC</t>
+          <t>APPLE INC</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.0133301597088575</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>541512</t>
+          <t>336111</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>714603</v>
+        <v>700841</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>3707</v>
+        <v>8892</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>DST SYSTEMS INC</t>
+          <t>RCM TECHNOLOGIES INC</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.000891265575774</v>
+        <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>334419</t>
+          <t>541512</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>723125</v>
+        <v>714603</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2668582551509522</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>7343</v>
+        <v>3707</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MICRON TECHNOLOGY INC</t>
+          <t>DST SYSTEMS INC</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.0063047283329069</v>
+        <v>0.000891265575774</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>519130</t>
+          <t>334419</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>751978</v>
+        <v>723125</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.2668582551509522</v>
       </c>
       <c r="C13" t="n">
-        <v>21238</v>
+        <v>7343</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>VICOR CORP</t>
+          <t>MICRON TECHNOLOGY INC</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.0063047283329069</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>334113</t>
+          <t>519130</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>789019</v>
+        <v>751978</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1523283981628243</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>12141</v>
+        <v>21238</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>MICROSOFT CORP</t>
+          <t>VICOR CORP</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.0242415703833103</v>
+        <v>0</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>999990</t>
+          <t>334113</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>792130</v>
+        <v>789019</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1666953516934278</v>
+        <v>0.1297716338097014</v>
       </c>
       <c r="C15" t="n">
-        <v>25320</v>
+        <v>12141</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>DATAWATCH CORP</t>
+          <t>MICROSOFT CORP</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>0.0242415703833103</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>511210</t>
+          <t>999990</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>794323</v>
+        <v>792130</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>0.1666953516934278</v>
       </c>
       <c r="C16" t="n">
-        <v>13440</v>
+        <v>25320</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>LEVEL 3 COMMUNICATIONS INC</t>
+          <t>DATAWATCH CORP</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.0006079027079977</v>
+        <v>0</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>519130</t>
+          <t>511210</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>796343</v>
+        <v>794323</v>
       </c>
       <c r="B17" t="n">
-        <v>0.427280084551808</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>12540</v>
+        <v>13440</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ADOBE SYSTEMS INC</t>
+          <t>LEVEL 3 COMMUNICATIONS INC</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.0239260476082563</v>
+        <v>0.0006079027079977</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>451110</t>
+          <t>519130</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>798354</v>
+        <v>796343</v>
       </c>
       <c r="B18" t="n">
-        <v>0.4491629633738837</v>
+        <v>0.3336805201127163</v>
       </c>
       <c r="C18" t="n">
-        <v>12635</v>
+        <v>12540</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>FISERV INC</t>
+          <t>ADOBE SYSTEMS INC</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.0002362949016969</v>
+        <v>0.0239260476082563</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>334111</t>
+          <t>451110</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>814547</v>
+        <v>798354</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1866117495426576</v>
+        <v>0.4491629633738837</v>
       </c>
       <c r="C19" t="n">
-        <v>13824</v>
+        <v>12635</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>FAIR ISAAC CORP</t>
+          <t>FISERV INC</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>0.0002362949016969</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>541512</t>
+          <t>334111</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>828146</v>
+        <v>814547</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>0.1588691915647324</v>
       </c>
       <c r="C20" t="n">
-        <v>28374</v>
+        <v>13824</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>INTERLINK ELECTRONICS</t>
+          <t>FAIR ISAAC CORP</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -905,23 +905,23 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>518210</t>
+          <t>541512</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>849547</v>
+        <v>828146</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>26012</v>
+        <v>28374</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>BLACK BOX CORP</t>
+          <t>INTERLINK ELECTRONICS</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -929,95 +929,95 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>511210</t>
+          <t>518210</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>857005</v>
+        <v>849547</v>
       </c>
       <c r="B22" t="n">
-        <v>0.5656636031473207</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>18699</v>
+        <v>26012</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>PARAMETRIC TECHNOLOGY CORP</t>
+          <t>BLACK BOX CORP</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.0051993066444993</v>
+        <v>0</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>334210</t>
+          <t>511210</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>858877</v>
+        <v>857005</v>
       </c>
       <c r="B23" t="n">
-        <v>0.4351165437101261</v>
+        <v>0.5656636031473207</v>
       </c>
       <c r="C23" t="n">
-        <v>20779</v>
+        <v>18699</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>CISCO SYSTEMS INC</t>
+          <t>PARAMETRIC TECHNOLOGY CORP</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.0061595761217176</v>
+        <v>0.0051993066444993</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>334210</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>866729</v>
+        <v>858877</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>0.4351165437101261</v>
       </c>
       <c r="C24" t="n">
-        <v>5349</v>
+        <v>20779</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>GROLIER INC</t>
+          <t>CISCO SYSTEMS INC</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>0.0061595761217176</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>519130</t>
+          <t>.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>882835</v>
+        <v>866729</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>64423</v>
+        <v>5349</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>DELTEK SYSTEMS INC</t>
+          <t>GROLIER INC</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1025,23 +1025,23 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>334413</t>
+          <t>519130</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>884144</v>
+        <v>882835</v>
       </c>
       <c r="B26" t="n">
-        <v>0.741461040838496</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>25138</v>
+        <v>64423</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>FORGENT NETWORKS INC</t>
+          <t>DELTEK SYSTEMS INC</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1049,95 +1049,95 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>541512</t>
+          <t>334413</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>896841</v>
+        <v>884144</v>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>0.741461040838496</v>
       </c>
       <c r="C27" t="n">
-        <v>27925</v>
+        <v>25138</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>AVID TECHNOLOGY INC</t>
+          <t>FORGENT NETWORKS INC</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.005167958792299</v>
+        <v>0</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>334220</t>
+          <t>541512</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>896878</v>
+        <v>896841</v>
       </c>
       <c r="B28" t="n">
-        <v>0.1407596238032312</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>27928</v>
+        <v>27925</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>INTUIT INC</t>
+          <t>AVID TECHNOLOGY INC</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.0137825421988964</v>
+        <v>0.005167958792299</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>337127</t>
+          <t>334220</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>903651</v>
+        <v>896878</v>
       </c>
       <c r="B29" t="n">
-        <v>0.6790482561804437</v>
+        <v>0.1413746127733945</v>
       </c>
       <c r="C29" t="n">
-        <v>28717</v>
+        <v>27928</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>INNODATA ISOGEN INC</t>
+          <t>INTUIT INC</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>0.0137825421988964</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>519130</t>
+          <t>337127</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>909494</v>
+        <v>903651</v>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>0.6790482561804437</v>
       </c>
       <c r="C30" t="n">
-        <v>62723</v>
+        <v>28717</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>TUCOWS INC</t>
+          <t>INNODATA ISOGEN INC</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1145,23 +1145,23 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>334413</t>
+          <t>519130</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>912093</v>
+        <v>909494</v>
       </c>
       <c r="B31" t="n">
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>29241</v>
+        <v>62723</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>JDS UNIPHASE CORP</t>
+          <t>TUCOWS INC</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1175,65 +1175,65 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>935036</v>
+        <v>912093</v>
       </c>
       <c r="B32" t="n">
-        <v>0.8919980393051106</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>31564</v>
+        <v>29241</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>TRNSACTN SYS ARCHTCTS  -CL A</t>
+          <t>JDS UNIPHASE CORP</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.0013386880746111</v>
+        <v>0</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>518210</t>
+          <t>334413</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>943034</v>
+        <v>935036</v>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>0.628501987066414</v>
       </c>
       <c r="C33" t="n">
-        <v>31775</v>
+        <v>31564</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>IMAGE SENSING SYSTEMS INC</t>
+          <t>TRNSACTN SYS ARCHTCTS  -CL A</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>0.0013386880746111</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>334419</t>
+          <t>518210</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1014111</v>
+        <v>943034</v>
       </c>
       <c r="B34" t="n">
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>7244</v>
+        <v>31775</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>MEMOREX CORP</t>
+          <t>IMAGE SENSING SYSTEMS INC</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1241,95 +1241,95 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>51121</t>
+          <t>334419</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1018724</v>
+        <v>1014111</v>
       </c>
       <c r="B35" t="n">
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>64768</v>
+        <v>7244</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>AMAZON.COM INC</t>
+          <t>MEMOREX CORP</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0.0122375879436731</v>
+        <v>0</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>51121</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1024478</v>
+        <v>1018724</v>
       </c>
       <c r="B36" t="n">
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>9203</v>
+        <v>64768</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ROCKWELL AUTOMATION</t>
+          <t>AMAZON.COM INC</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.0007662835414521</v>
+        <v>0.0122375879436731</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>541512</t>
+          <t>.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1029744</v>
+        <v>1024478</v>
       </c>
       <c r="B37" t="n">
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>109186</v>
+        <v>9203</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>SONIC FOUNDRY INC</t>
+          <t>ROCKWELL AUTOMATION</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>0.0007662835414521</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>334119</t>
+          <t>541512</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1036188</v>
+        <v>1029744</v>
       </c>
       <c r="B38" t="n">
-        <v>0.513379092450063</v>
+        <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>65226</v>
+        <v>109186</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>QAD INC</t>
+          <t>SONIC FOUNDRY INC</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1337,23 +1337,23 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>511210</t>
+          <t>334119</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1038222</v>
+        <v>1036188</v>
       </c>
       <c r="B39" t="n">
-        <v>0</v>
+        <v>0.1105707743217683</v>
       </c>
       <c r="C39" t="n">
-        <v>64850</v>
+        <v>65226</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>REIS INC</t>
+          <t>QAD INC</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1361,167 +1361,167 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>519130</t>
+          <t>511210</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1065280</v>
+        <v>1038222</v>
       </c>
       <c r="B40" t="n">
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>147579</v>
+        <v>64850</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>NETFLIX INC</t>
+          <t>REIS INC</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0.0133382733911275</v>
+        <v>0</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>332721</t>
+          <t>519130</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1078099</v>
+        <v>1065280</v>
       </c>
       <c r="B41" t="n">
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>121662</v>
+        <v>147579</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>QUEPASA CORP</t>
+          <t>NETFLIX INC</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>0.0133382733911275</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>541512</t>
+          <t>332721</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1087423</v>
+        <v>1078099</v>
       </c>
       <c r="B42" t="n">
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>122841</v>
+        <v>121662</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>RED HAT INC</t>
+          <t>QUEPASA CORP</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.0047281323932111</v>
+        <v>0</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>334119</t>
+          <t>541512</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1108524</v>
+        <v>1087423</v>
       </c>
       <c r="B43" t="n">
-        <v>0.2001972116607018</v>
+        <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>157855</v>
+        <v>122841</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>SALESFORCE.COM INC</t>
+          <t>RED HAT INC</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.0081739416345953</v>
+        <v>0.0047281323932111</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>325414</t>
+          <t>334119</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1130713</v>
+        <v>1108524</v>
       </c>
       <c r="B44" t="n">
-        <v>0.3688601527724288</v>
+        <v>0.2001972116607018</v>
       </c>
       <c r="C44" t="n">
-        <v>147868</v>
+        <v>157855</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>OVERSTOCK.COM INC</t>
+          <t>SALESFORCE.COM INC</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.015358361415565</v>
+        <v>0.0081739416345953</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>511210</t>
+          <t>325414</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1157817</v>
+        <v>1130713</v>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
+        <v>0.3688601527724288</v>
       </c>
       <c r="C45" t="n">
-        <v>149360</v>
+        <v>147868</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>HOSTING SITE NETWORK INC</t>
+          <t>OVERSTOCK.COM INC</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>0.015358361415565</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>334413</t>
+          <t>511210</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1296445</v>
+        <v>1157817</v>
       </c>
       <c r="B46" t="n">
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>160913</v>
+        <v>149360</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>ORMAT TECHNOLOGIES INC</t>
+          <t>HOSTING SITE NETWORK INC</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1529,71 +1529,71 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>511210</t>
+          <t>334413</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1341439</v>
+        <v>1296445</v>
       </c>
       <c r="B47" t="n">
-        <v>0.5324551103999438</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>12142</v>
+        <v>160913</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ORACLE CORP</t>
+          <t>ORMAT TECHNOLOGIES INC</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.0071220458485186</v>
+        <v>0</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>561990</t>
+          <t>511210</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1561880</v>
+        <v>1341439</v>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>0.3457255015383973</v>
       </c>
       <c r="C48" t="n">
-        <v>114242</v>
+        <v>12142</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>WHITNEY INFORMATION NET INC</t>
+          <t>ORACLE CORP</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>0.0071220458485186</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>541519</t>
+          <t>561990</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1633917</v>
+        <v>1561880</v>
       </c>
       <c r="B49" t="n">
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>145471</v>
+        <v>114242</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>PAYPAL INC</t>
+          <t>WHITNEY INFORMATION NET INC</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1601,31 +1601,79 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>334310</t>
+          <t>541519</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
+        <v>1633917</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>145471</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>PAYPAL INC</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>334310</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
         <v>1645494</v>
       </c>
-      <c r="B50" t="n">
-        <v>0</v>
-      </c>
-      <c r="C50" t="n">
+      <c r="B51" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" t="n">
         <v>28853</v>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>ARRIS GROUP INC</t>
         </is>
       </c>
-      <c r="E50" t="n">
+      <c r="E51" t="n">
         <v>0.0011198208667337</v>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>511210</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1652044</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.4065383566387364</v>
+      </c>
+      <c r="C52" t="n">
+        <v>160329</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>GOOGLE INC</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>0.0297704450786113</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>334111</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Filtered out some garbage markup that was squeezing through
</commit_message>
<xml_diff>
--- a/Batch_A_Report.xlsx
+++ b/Batch_A_Report.xlsx
@@ -458,7 +458,7 @@
         <v>6281</v>
       </c>
       <c r="B2" t="n">
-        <v>0.03101405352916946</v>
+        <v>0.03675</v>
       </c>
       <c r="C2" t="n">
         <v>1632</v>
@@ -530,7 +530,7 @@
         <v>50863</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2443607110705934</v>
+        <v>5.524925000000001</v>
       </c>
       <c r="C5" t="n">
         <v>6008</v>
@@ -626,7 +626,7 @@
         <v>106040</v>
       </c>
       <c r="B9" t="n">
-        <v>0.63974640383283</v>
+        <v>0.1716</v>
       </c>
       <c r="C9" t="n">
         <v>11399</v>
@@ -722,7 +722,7 @@
         <v>723125</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2668582551509522</v>
+        <v>2.2212</v>
       </c>
       <c r="C13" t="n">
         <v>7343</v>
@@ -770,7 +770,7 @@
         <v>789019</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1297716338097014</v>
+        <v>12.683135</v>
       </c>
       <c r="C15" t="n">
         <v>12141</v>
@@ -794,7 +794,7 @@
         <v>792130</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1666953516934278</v>
+        <v>1.904905</v>
       </c>
       <c r="C16" t="n">
         <v>25320</v>
@@ -842,7 +842,7 @@
         <v>796343</v>
       </c>
       <c r="B18" t="n">
-        <v>0.3336805201127163</v>
+        <v>2.822072</v>
       </c>
       <c r="C18" t="n">
         <v>12540</v>
@@ -866,7 +866,7 @@
         <v>798354</v>
       </c>
       <c r="B19" t="n">
-        <v>0.4491629633738837</v>
+        <v>0.126225</v>
       </c>
       <c r="C19" t="n">
         <v>12635</v>
@@ -890,7 +890,7 @@
         <v>814547</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1588691915647324</v>
+        <v>11.7016</v>
       </c>
       <c r="C20" t="n">
         <v>13824</v>
@@ -962,7 +962,7 @@
         <v>857005</v>
       </c>
       <c r="B23" t="n">
-        <v>0.5656636031473207</v>
+        <v>2.34657</v>
       </c>
       <c r="C23" t="n">
         <v>18699</v>
@@ -986,7 +986,7 @@
         <v>858877</v>
       </c>
       <c r="B24" t="n">
-        <v>0.4351165437101261</v>
+        <v>3.46575</v>
       </c>
       <c r="C24" t="n">
         <v>20779</v>
@@ -1058,7 +1058,7 @@
         <v>884144</v>
       </c>
       <c r="B27" t="n">
-        <v>0.741461040838496</v>
+        <v>0.006000000000000002</v>
       </c>
       <c r="C27" t="n">
         <v>25138</v>
@@ -1106,7 +1106,7 @@
         <v>896878</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1413746127733945</v>
+        <v>2.021495</v>
       </c>
       <c r="C29" t="n">
         <v>27928</v>
@@ -1130,7 +1130,7 @@
         <v>903651</v>
       </c>
       <c r="B30" t="n">
-        <v>0.6790482561804437</v>
+        <v>0.425425</v>
       </c>
       <c r="C30" t="n">
         <v>28717</v>
@@ -1202,7 +1202,7 @@
         <v>935036</v>
       </c>
       <c r="B33" t="n">
-        <v>0.628501987066414</v>
+        <v>0.8747999999999999</v>
       </c>
       <c r="C33" t="n">
         <v>31564</v>
@@ -1346,7 +1346,7 @@
         <v>1036188</v>
       </c>
       <c r="B39" t="n">
-        <v>0.1105707743217683</v>
+        <v>0.277725</v>
       </c>
       <c r="C39" t="n">
         <v>65226</v>
@@ -1466,7 +1466,7 @@
         <v>1108524</v>
       </c>
       <c r="B44" t="n">
-        <v>0.2001972116607018</v>
+        <v>6.219109</v>
       </c>
       <c r="C44" t="n">
         <v>157855</v>
@@ -1490,7 +1490,7 @@
         <v>1130713</v>
       </c>
       <c r="B45" t="n">
-        <v>0.3688601527724288</v>
+        <v>0.37315</v>
       </c>
       <c r="C45" t="n">
         <v>147868</v>
@@ -1562,7 +1562,7 @@
         <v>1341439</v>
       </c>
       <c r="B48" t="n">
-        <v>0.3457255015383973</v>
+        <v>1.86171</v>
       </c>
       <c r="C48" t="n">
         <v>12142</v>
@@ -1658,7 +1658,7 @@
         <v>1652044</v>
       </c>
       <c r="B52" t="n">
-        <v>0.4065383566387364</v>
+        <v>4.041088</v>
       </c>
       <c r="C52" t="n">
         <v>160329</v>

</xml_diff>